<commit_message>
adding unathorized page for unathorized users
</commit_message>
<xml_diff>
--- a/app/resources/canvas/groupe-canva.xlsx
+++ b/app/resources/canvas/groupe-canva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ABS-ISTA\app\resources\canvas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03CF41D-FC2E-4326-8788-E49FB28F7637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FCBC25-7A5E-414D-96E3-FF6C231C8B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Groupe</t>
   </si>
   <si>
-    <t>Filière</t>
+    <t>Gestionnaire</t>
+  </si>
+  <si>
+    <t>la valeur par défaut de Gestionnaire = 1</t>
+  </si>
+  <si>
+    <t>Filiere</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +59,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,15 +102,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -114,11 +166,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AFACD98-3970-4077-8154-94E50ACB833B}" name="Table1" displayName="Table1" ref="A1:B2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B2" xr:uid="{1AFACD98-3970-4077-8154-94E50ACB833B}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AFACD98-3970-4077-8154-94E50ACB833B}" name="Table1" displayName="Table1" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C2" xr:uid="{1AFACD98-3970-4077-8154-94E50ACB833B}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AEC9E63E-4822-4939-BBD3-9EEB4F84567C}" name="Groupe"/>
-    <tableColumn id="2" xr3:uid="{E6BE985D-0B6E-458A-B049-01C68C00C63C}" name="Filière"/>
+    <tableColumn id="2" xr3:uid="{E6BE985D-0B6E-458A-B049-01C68C00C63C}" name="Filiere"/>
+    <tableColumn id="3" xr3:uid="{0BCB2A28-838A-402D-AAEB-52C5E9997D50}" name="Gestionnaire"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -387,24 +440,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>